<commit_message>
Atualizações Ata e Gestão de Riscos
</commit_message>
<xml_diff>
--- a/Gestão de Riscos.xlsx
+++ b/Gestão de Riscos.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Projeto e Inovação\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Projeto e Inovação\Documentacao-ArtVisionTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EDDC0790-8AF4-40F6-924D-69DF237C6DB2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DBEE86-E9C2-47FF-9AC8-5A31484083F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,20 +18,16 @@
     <sheet name="Gráfico1" sheetId="9" r:id="rId3"/>
     <sheet name="Gráfico5" sheetId="13" r:id="rId4"/>
     <sheet name="Gráfico4" sheetId="12" r:id="rId5"/>
-    <sheet name="EXAMPLE Product Backlog" sheetId="8" r:id="rId6"/>
-    <sheet name="BLANK Product Backlog" sheetId="7" r:id="rId7"/>
-    <sheet name="- Disclaimer -" sheetId="3" r:id="rId8"/>
+    <sheet name="Gestão de Riscos" sheetId="8" r:id="rId6"/>
   </sheets>
   <externalReferences>
-    <externalReference r:id="rId9"/>
-    <externalReference r:id="rId10"/>
+    <externalReference r:id="rId7"/>
+    <externalReference r:id="rId8"/>
   </externalReferences>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="6">'BLANK Product Backlog'!$B$1:$I$18</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="5">'EXAMPLE Product Backlog'!$B$1:$H$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="5">'Gestão de Riscos'!$B$1:$H$8</definedName>
     <definedName name="Interval">'[1]12-Month Sales Forecast'!#REF!</definedName>
     <definedName name="ScheduleStart">'[1]12-Month Sales Forecast'!#REF!</definedName>
-    <definedName name="Type" localSheetId="6">'[2]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type" localSheetId="5">'[2]Maintenance Work Order'!#REF!</definedName>
     <definedName name="Type">'[2]Maintenance Work Order'!#REF!</definedName>
   </definedNames>
@@ -48,75 +44,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="55">
-  <si>
-    <t xml:space="preserve">PRODUCT BACKLOG REPORT </t>
-  </si>
-  <si>
-    <t>Classificação</t>
-  </si>
-  <si>
-    <t>STATUS</t>
-  </si>
-  <si>
-    <t>Essencial</t>
-  </si>
-  <si>
-    <t>Complete</t>
-  </si>
-  <si>
-    <t>Not Started</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Importante</t>
-  </si>
-  <si>
-    <t>Overdue</t>
-  </si>
-  <si>
-    <t>Desejável</t>
-  </si>
-  <si>
-    <t>Medium</t>
-  </si>
-  <si>
-    <t>On Hold</t>
-  </si>
-  <si>
-    <t>High</t>
-  </si>
-  <si>
-    <t>Low</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PRODUCT BACKLOG TEMPLATE </t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
   <si>
     <t>ID</t>
-  </si>
-  <si>
-    <t>AS A …</t>
-  </si>
-  <si>
-    <t>I WANT TO …</t>
-  </si>
-  <si>
-    <t>SO THAT …</t>
-  </si>
-  <si>
-    <t>PRIORITY</t>
-  </si>
-  <si>
-    <t>SPRINT</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Any articles, templates, or information provided by Smartsheet on the website are for reference only. While we strive to keep the information up to date and correct, we make no representations or warranties of any kind, express or implied, about the completeness, accuracy, reliability, suitability, or availability with respect to the website or the information, articles, templates, or related graphics contained on the website. Any reliance you place on such information is therefore strictly at your own risk. </t>
   </si>
   <si>
     <t>Descrição do Risco</t>
@@ -229,10 +159,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
-  </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -267,12 +194,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -325,31 +246,6 @@
       <family val="1"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Century Gothic"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="0"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <color theme="1" tint="0.34998626667073579"/>
-      <name val="Century Gothic"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Century Gothic"/>
@@ -361,25 +257,20 @@
       <name val="Century Gothic"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Century Gothic"/>
+      <family val="1"/>
+    </font>
   </fonts>
-  <fills count="13">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -395,31 +286,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="1" tint="0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="3" tint="-0.499984740745262"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -436,33 +303,9 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="2">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thick">
-        <color theme="0" tint="-0.34998626667073579"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -483,43 +326,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.24994659260841701"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -531,121 +337,69 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="9"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="7" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="12" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1" readingOrder="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="8" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="17" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="13" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -659,302 +413,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
-  <dxfs count="42">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81D6F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00BD32"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2D2D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81D6F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00BD32"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2D2D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF81D6F0"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00BD32"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFD2D2D2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFAAEEE6"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium7"/>
   <colors>
     <mruColors>
@@ -1038,112 +497,110 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'EXAMPLE Product Backlog'!$C$1:$H$8</c:f>
+              <c:f>'Gestão de Riscos'!$C$1:$H$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Escopo confuso/não bem definido</c:v>
-                  </c:pt>
                   <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de conhecimento</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>9</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Perder um integrante na equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Descrição do Risco</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Probabilidade (P)</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Impacto (I)</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Fator de Risco
-        (P x I)</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
                     <c:v>Ação
 -Evitar
 -Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Fator de Risco
+        (P x I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Impacto (I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Probabilidade (P)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Descrição do Risco</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Perder um integrante na equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Falta de conhecimento</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Escopo confuso/não bem definido</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1421,112 +878,110 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'EXAMPLE Product Backlog'!$C$1:$H$8</c:f>
+              <c:f>'Gestão de Riscos'!$C$1:$H$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Escopo confuso/não bem definido</c:v>
-                  </c:pt>
                   <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de conhecimento</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>9</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Perder um integrante na equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Descrição do Risco</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Probabilidade (P)</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Impacto (I)</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Fator de Risco
-        (P x I)</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
                     <c:v>Ação
 -Evitar
 -Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Fator de Risco
+        (P x I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Impacto (I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Probabilidade (P)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Descrição do Risco</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Perder um integrante na equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Falta de conhecimento</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Escopo confuso/não bem definido</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -1804,112 +1259,110 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'EXAMPLE Product Backlog'!$C$1:$H$8</c:f>
+              <c:f>'Gestão de Riscos'!$C$1:$H$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Escopo confuso/não bem definido</c:v>
-                  </c:pt>
                   <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de conhecimento</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>9</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Perder um integrante na equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Descrição do Risco</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Probabilidade (P)</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Impacto (I)</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Fator de Risco
-        (P x I)</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
                     <c:v>Ação
 -Evitar
 -Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Fator de Risco
+        (P x I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Impacto (I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Probabilidade (P)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Descrição do Risco</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Perder um integrante na equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Falta de conhecimento</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Escopo confuso/não bem definido</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2187,112 +1640,110 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'EXAMPLE Product Backlog'!$C$1:$H$8</c:f>
+              <c:f>'Gestão de Riscos'!$C$1:$H$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Escopo confuso/não bem definido</c:v>
-                  </c:pt>
                   <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de conhecimento</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>9</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Perder um integrante na equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Descrição do Risco</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Probabilidade (P)</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Impacto (I)</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Fator de Risco
-        (P x I)</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
                     <c:v>Ação
 -Evitar
 -Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Fator de Risco
+        (P x I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Impacto (I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Probabilidade (P)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Descrição do Risco</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Perder um integrante na equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Falta de conhecimento</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Escopo confuso/não bem definido</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -2570,112 +2021,110 @@
           <c:invertIfNegative val="0"/>
           <c:cat>
             <c:multiLvlStrRef>
-              <c:f>'EXAMPLE Product Backlog'!$C$1:$H$8</c:f>
+              <c:f>'Gestão de Riscos'!$C$1:$H$8</c:f>
               <c:multiLvlStrCache>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Escopo confuso/não bem definido</c:v>
-                  </c:pt>
                   <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de conhecimento</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>2</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>6</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>9</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Evitar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Perder um integrante na equipe</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>1</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>3</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
-                    <c:v>Mitigar</c:v>
-                  </c:pt>
-                </c:lvl>
-                <c:lvl>
-                  <c:pt idx="0">
-                    <c:v>Descrição do Risco</c:v>
-                  </c:pt>
-                  <c:pt idx="2">
-                    <c:v>Probabilidade (P)</c:v>
-                  </c:pt>
-                  <c:pt idx="3">
-                    <c:v>Impacto (I)</c:v>
-                  </c:pt>
-                  <c:pt idx="4">
-                    <c:v>Fator de Risco
-        (P x I)</c:v>
-                  </c:pt>
-                  <c:pt idx="5">
                     <c:v>Ação
 -Evitar
 -Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Mitigar</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Evitar</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Fator de Risco
+        (P x I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>9</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>6</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Impacto (I)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>2</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Probabilidade (P)</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>1</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>2</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>3</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>1</c:v>
+                  </c:pt>
+                </c:lvl>
+                <c:lvl>
+                  <c:pt idx="2">
+                    <c:v>Descrição do Risco</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>Perder um integrante na equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>Dificuldade de comunicação entre os membros da equipe</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>Falta de comprometimento com as entregas do Projeto</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>Falta de conhecimento</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>Escopo confuso/não bem definido</c:v>
                   </c:pt>
                 </c:lvl>
               </c:multiLvlStrCache>
@@ -6121,11 +5570,11 @@
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K13"/>
+  <dimension ref="A1:L13"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H11" sqref="H11"/>
+      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6137,740 +5586,252 @@
     <col min="8" max="8" width="11.59765625" style="1" customWidth="1"/>
     <col min="9" max="9" width="30.69921875" style="1" customWidth="1"/>
     <col min="10" max="10" width="3.09765625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="1" customWidth="1"/>
-    <col min="12" max="16384" width="10.8984375" style="1"/>
+    <col min="11" max="16384" width="10.8984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="29" t="s">
-        <v>40</v>
+    <row r="1" spans="1:12" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="6"/>
+      <c r="B1" s="17" t="s">
+        <v>18</v>
       </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
     </row>
-    <row r="2" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30"/>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
+    <row r="2" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="18"/>
+      <c r="C2" s="18"/>
+      <c r="D2" s="18"/>
     </row>
-    <row r="3" spans="1:11" s="8" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="14" t="s">
+    <row r="3" spans="1:12" s="4" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3"/>
+      <c r="B3" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="D3" s="19"/>
+      <c r="E3" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="10">
+        <v>1</v>
+      </c>
+      <c r="C4" s="20" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="21"/>
+      <c r="E4" s="7">
+        <v>1</v>
+      </c>
+      <c r="F4" s="7">
+        <v>3</v>
+      </c>
+      <c r="G4" s="11">
+        <v>3</v>
+      </c>
+      <c r="H4" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="12" t="s">
+        <v>14</v>
+      </c>
+      <c r="L4" s="23"/>
+    </row>
+    <row r="5" spans="1:12" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="10">
+        <v>2</v>
+      </c>
+      <c r="C5" s="22" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="22"/>
+      <c r="E5" s="7">
+        <v>3</v>
+      </c>
+      <c r="F5" s="7">
+        <v>3</v>
+      </c>
+      <c r="G5" s="11">
+        <v>9</v>
+      </c>
+      <c r="H5" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="12" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="10">
+        <v>3</v>
+      </c>
+      <c r="C6" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6" s="22"/>
+      <c r="E6" s="7">
+        <v>2</v>
+      </c>
+      <c r="F6" s="7">
+        <v>3</v>
+      </c>
+      <c r="G6" s="11">
+        <v>6</v>
+      </c>
+      <c r="H6" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="10">
+        <v>4</v>
+      </c>
+      <c r="C7" s="22" t="s">
         <v>16</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="D7" s="22"/>
+      <c r="E7" s="7">
+        <v>3</v>
+      </c>
+      <c r="F7" s="7">
+        <v>1</v>
+      </c>
+      <c r="G7" s="11">
+        <v>3</v>
+      </c>
+      <c r="H7" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="I7" s="12" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
+        <v>5</v>
+      </c>
+      <c r="C8" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="22"/>
+      <c r="E8" s="7">
+        <v>1</v>
+      </c>
+      <c r="F8" s="7">
+        <v>2</v>
+      </c>
+      <c r="G8" s="11">
+        <v>2</v>
+      </c>
+      <c r="H8" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3"/>
+      <c r="B9" s="8" t="s">
+        <v>3</v>
+      </c>
+      <c r="C9" s="9"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+    </row>
+    <row r="10" spans="1:12" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="9"/>
+    </row>
+    <row r="11" spans="1:12" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2</v>
+      </c>
+      <c r="D11" s="15">
+        <v>4</v>
+      </c>
+      <c r="E11" s="16">
+        <v>6</v>
+      </c>
+      <c r="F11" s="9"/>
+    </row>
+    <row r="12" spans="1:12" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B12" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="31"/>
-      <c r="E3" s="15" t="s">
+      <c r="C12" s="14">
+        <v>1</v>
+      </c>
+      <c r="D12" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="9"/>
+    </row>
+    <row r="13" spans="1:12" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3"/>
+      <c r="B13" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="F3" s="15" t="s">
-        <v>30</v>
+      <c r="D13" s="9" t="s">
+        <v>25</v>
       </c>
-      <c r="G3" s="38" t="s">
-        <v>27</v>
-      </c>
-      <c r="H3" s="14" t="s">
+      <c r="E13" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I3" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23">
-        <v>1</v>
-      </c>
-      <c r="C4" s="37" t="s">
-        <v>29</v>
-      </c>
-      <c r="D4" s="32"/>
-      <c r="E4" s="13">
-        <v>1</v>
-      </c>
-      <c r="F4" s="13">
-        <v>3</v>
-      </c>
-      <c r="G4" s="25">
-        <v>3</v>
-      </c>
-      <c r="H4" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I4" s="27" t="s">
-        <v>36</v>
-      </c>
-      <c r="K4" s="18" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23">
-        <v>2</v>
-      </c>
-      <c r="C5" s="28" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" s="28"/>
-      <c r="E5" s="13">
-        <v>3</v>
-      </c>
-      <c r="F5" s="13">
-        <v>3</v>
-      </c>
-      <c r="G5" s="25">
-        <v>9</v>
-      </c>
-      <c r="H5" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23">
-        <v>3</v>
-      </c>
-      <c r="C6" s="28" t="s">
-        <v>35</v>
-      </c>
-      <c r="D6" s="28"/>
-      <c r="E6" s="13">
-        <v>2</v>
-      </c>
-      <c r="F6" s="13">
-        <v>3</v>
-      </c>
-      <c r="G6" s="25">
-        <v>6</v>
-      </c>
-      <c r="H6" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I6" s="27" t="s">
-        <v>37</v>
-      </c>
-      <c r="K6" s="20" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23">
-        <v>4</v>
-      </c>
-      <c r="C7" s="28" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="28"/>
-      <c r="E7" s="13">
-        <v>3</v>
-      </c>
-      <c r="F7" s="13">
-        <v>1</v>
-      </c>
-      <c r="G7" s="25">
-        <v>3</v>
-      </c>
-      <c r="H7" s="25" t="s">
-        <v>31</v>
-      </c>
-      <c r="I7" s="27" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23">
-        <v>5</v>
-      </c>
-      <c r="C8" s="28" t="s">
-        <v>41</v>
-      </c>
-      <c r="D8" s="28"/>
-      <c r="E8" s="13">
-        <v>1</v>
-      </c>
-      <c r="F8" s="13">
-        <v>2</v>
-      </c>
-      <c r="G8" s="25">
-        <v>2</v>
-      </c>
-      <c r="H8" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="I8" s="27" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="9" spans="1:11" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="7"/>
-      <c r="B9" s="14" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-    </row>
-    <row r="10" spans="1:11" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="23" t="s">
-        <v>43</v>
-      </c>
-      <c r="C10" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="41" t="s">
-        <v>52</v>
-      </c>
-      <c r="E10" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:11" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23" t="s">
-        <v>44</v>
-      </c>
-      <c r="C11" s="39">
-        <v>2</v>
-      </c>
-      <c r="D11" s="40">
-        <v>4</v>
-      </c>
-      <c r="E11" s="41">
-        <v>6</v>
-      </c>
-      <c r="F11" s="15"/>
-    </row>
-    <row r="12" spans="1:11" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23" t="s">
-        <v>45</v>
-      </c>
-      <c r="C12" s="39">
-        <v>1</v>
-      </c>
-      <c r="D12" s="39" t="s">
-        <v>54</v>
-      </c>
-      <c r="E12" s="40" t="s">
-        <v>53</v>
-      </c>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:11" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="7"/>
-      <c r="B13" s="14" t="s">
-        <v>49</v>
-      </c>
-      <c r="C13" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="E13" s="15" t="s">
-        <v>48</v>
-      </c>
-      <c r="F13" s="15"/>
+      <c r="F13" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="C7:D7"/>
+    <mergeCell ref="C8:D8"/>
     <mergeCell ref="B1:D1"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="C8:D8"/>
   </mergeCells>
-  <conditionalFormatting sqref="K4:K6">
-    <cfRule type="containsText" dxfId="33" priority="57" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",K4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="32" priority="58" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",K4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="31" priority="59" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",K4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EC855CE-A1B3-4462-93F9-7DF8769B412F}">
-  <sheetPr>
-    <tabColor theme="3" tint="0.79998168889431442"/>
-    <pageSetUpPr fitToPage="1"/>
-  </sheetPr>
-  <dimension ref="A1:M19"/>
-  <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="3.09765625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="9.3984375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="29.3984375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="11.59765625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="61.09765625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="36" style="1" customWidth="1"/>
-    <col min="7" max="9" width="15.59765625" style="1" customWidth="1"/>
-    <col min="10" max="10" width="3.09765625" style="1" customWidth="1"/>
-    <col min="11" max="11" width="15.59765625" style="1" customWidth="1"/>
-    <col min="12" max="12" width="3.09765625" style="1" customWidth="1"/>
-    <col min="13" max="13" width="15.59765625" style="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.8984375" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:13" s="9" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="10"/>
-      <c r="B1" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="C1" s="29"/>
-      <c r="D1" s="29"/>
-      <c r="E1" s="29"/>
-    </row>
-    <row r="2" spans="1:13" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="30" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="30"/>
-      <c r="E2" s="30"/>
-    </row>
-    <row r="3" spans="1:13" s="8" customFormat="1" ht="32.1" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="7"/>
-      <c r="B3" s="14" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" s="33" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" s="33"/>
-      <c r="E3" s="15" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="15" t="s">
-        <v>19</v>
-      </c>
-      <c r="G3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>21</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="K3" s="21" t="s">
-        <v>2</v>
-      </c>
-      <c r="M3" s="21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23"/>
-      <c r="C4" s="28"/>
-      <c r="D4" s="28"/>
-      <c r="E4" s="12"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4" s="25">
-        <v>0</v>
-      </c>
-      <c r="I4" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="K4" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="M4" s="18" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="23"/>
-      <c r="C5" s="28"/>
-      <c r="D5" s="28"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="13"/>
-      <c r="G5" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5" s="25">
-        <v>0</v>
-      </c>
-      <c r="I5" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="K5" s="17" t="s">
-        <v>6</v>
-      </c>
-      <c r="M5" s="19" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23"/>
-      <c r="C6" s="28"/>
-      <c r="D6" s="28"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H6" s="25">
-        <v>0</v>
-      </c>
-      <c r="I6" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="K6" s="17" t="s">
-        <v>4</v>
-      </c>
-      <c r="M6" s="20" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="23"/>
-      <c r="C7" s="28"/>
-      <c r="D7" s="28"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="25">
-        <v>0</v>
-      </c>
-      <c r="I7" s="22" t="s">
-        <v>11</v>
-      </c>
-      <c r="K7" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="28"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="13"/>
-      <c r="G8" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H8" s="25">
-        <v>0</v>
-      </c>
-      <c r="I8" s="22" t="s">
-        <v>4</v>
-      </c>
-      <c r="K8" s="11" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="23"/>
-      <c r="C9" s="28"/>
-      <c r="D9" s="28"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H9" s="25">
-        <v>0</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="23"/>
-      <c r="C10" s="28"/>
-      <c r="D10" s="28"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H10" s="25">
-        <v>0</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="23"/>
-      <c r="C11" s="28"/>
-      <c r="D11" s="28"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H11" s="25">
-        <v>0</v>
-      </c>
-      <c r="I11" s="22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="23"/>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H12" s="25">
-        <v>0</v>
-      </c>
-      <c r="I12" s="22" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="23"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="28"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H13" s="25">
-        <v>0</v>
-      </c>
-      <c r="I13" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="23"/>
-      <c r="C14" s="28"/>
-      <c r="D14" s="28"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="22" t="s">
-        <v>12</v>
-      </c>
-      <c r="H14" s="25">
-        <v>0</v>
-      </c>
-      <c r="I14" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="23"/>
-      <c r="C15" s="28"/>
-      <c r="D15" s="28"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H15" s="25">
-        <v>0</v>
-      </c>
-      <c r="I15" s="22" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="23"/>
-      <c r="C16" s="28"/>
-      <c r="D16" s="28"/>
-      <c r="E16" s="12"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="H16" s="25">
-        <v>0</v>
-      </c>
-      <c r="I16" s="22" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="23"/>
-      <c r="C17" s="28"/>
-      <c r="D17" s="28"/>
-      <c r="E17" s="12"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="22" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="25">
-        <v>0</v>
-      </c>
-      <c r="I17" s="22" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" ht="24.9" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="34" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="35"/>
-      <c r="F18" s="35"/>
-      <c r="G18" s="36"/>
-      <c r="H18" s="26">
-        <f>SUM(H4:H17)</f>
-        <v>0</v>
-      </c>
-      <c r="I18" s="24"/>
-    </row>
-    <row r="19" spans="1:9" s="5" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="6"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="6"/>
-    </row>
-  </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C16:D16"/>
-    <mergeCell ref="C17:D17"/>
-    <mergeCell ref="B18:G18"/>
-    <mergeCell ref="C10:D10"/>
-    <mergeCell ref="C15:D15"/>
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:D14"/>
-    <mergeCell ref="C7:D7"/>
-    <mergeCell ref="B1:E1"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="C6:D6"/>
-  </mergeCells>
-  <conditionalFormatting sqref="G4:G17">
-    <cfRule type="containsText" dxfId="15" priority="6" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",G4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="14" priority="7" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",G4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="13" priority="8" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",G4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I4:I17">
-    <cfRule type="containsText" dxfId="12" priority="1" operator="containsText" text="Overdue">
-      <formula>NOT(ISERROR(SEARCH("Overdue",I4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="11" priority="2" operator="containsText" text="On Hold">
-      <formula>NOT(ISERROR(SEARCH("On Hold",I4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="10" priority="3" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",I4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="9" priority="4" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",I4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="8" priority="5" operator="containsText" text="Not Started">
-      <formula>NOT(ISERROR(SEARCH("Not Started",I4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K4:K8">
-    <cfRule type="containsText" dxfId="7" priority="12" operator="containsText" text="Overdue">
-      <formula>NOT(ISERROR(SEARCH("Overdue",K4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="13" operator="containsText" text="On Hold">
-      <formula>NOT(ISERROR(SEARCH("On Hold",K4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="14" operator="containsText" text="Complete">
-      <formula>NOT(ISERROR(SEARCH("Complete",K4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="4" priority="15" operator="containsText" text="In Progress">
-      <formula>NOT(ISERROR(SEARCH("In Progress",K4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="3" priority="16" operator="containsText" text="Not Started">
-      <formula>NOT(ISERROR(SEARCH("Not Started",K4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M4:M6">
-    <cfRule type="containsText" dxfId="2" priority="9" operator="containsText" text="Low">
-      <formula>NOT(ISERROR(SEARCH("Low",M4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="1" priority="10" operator="containsText" text="Medium">
-      <formula>NOT(ISERROR(SEARCH("Medium",M4)))</formula>
-    </cfRule>
-    <cfRule type="containsText" dxfId="0" priority="11" operator="containsText" text="High">
-      <formula>NOT(ISERROR(SEARCH("High",M4)))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="I4:I17" xr:uid="{27263ABE-4B1D-4BFC-B079-C0425B7FF5F8}">
-      <formula1>$K$4:$K$8</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G4:G17" xr:uid="{C9161828-3D0A-4354-8FF9-0588FF283786}">
-      <formula1>$M$4:$M$6</formula1>
-    </dataValidation>
-  </dataValidations>
-  <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
-  <pageSetup scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <sheetPr>
-    <tabColor theme="1" tint="0.34998626667073579"/>
-  </sheetPr>
-  <dimension ref="B1:B2"/>
-  <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="W47" sqref="W47"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="3.3984375" style="3" customWidth="1"/>
-    <col min="2" max="2" width="88.3984375" style="3" customWidth="1"/>
-    <col min="3" max="16384" width="10.8984375" style="3"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:2" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:2" ht="105" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -6884,6 +5845,14 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678EE90E01C1554D81095FA0DFA567B7" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="012a7ac64c29fded4fe9435d797e27e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e7a52f9-5c66-44a9-86f3-38766607b952" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05da1342c08114b6330d010208ca11d1" ns3:_="">
     <xsd:import namespace="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
@@ -7033,14 +6002,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD8DBBE0-27BD-4D68-870A-6C9CFB0BB6CC}">
   <ds:schemaRefs>
@@ -7050,6 +6011,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3B143F-61D5-4FE7-AF30-9937B84882D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E784C7A-215E-4BC6-9503-8564823AE577}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7065,14 +6036,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3B143F-61D5-4FE7-AF30-9937B84882D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Atualizar Gestão de Riscos
</commit_message>
<xml_diff>
--- a/Gestão de Riscos.xlsx
+++ b/Gestão de Riscos.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\Projeto e Inovação\Documentacao-ArtVisionTech\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DBEE86-E9C2-47FF-9AC8-5A31484083F8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75D670EB-794C-4766-BF66-66755BA67BE9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" tabRatio="500" firstSheet="4" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="28">
   <si>
     <t>ID</t>
   </si>
@@ -138,21 +138,6 @@
   </si>
   <si>
     <t>Probabilidade</t>
-  </si>
-  <si>
-    <t>3 (1)</t>
-  </si>
-  <si>
-    <t>9 (2)</t>
-  </si>
-  <si>
-    <t>6 (3)</t>
-  </si>
-  <si>
-    <t>3 (4)</t>
-  </si>
-  <si>
-    <t>2 (5)</t>
   </si>
 </sst>
 </file>
@@ -381,6 +366,10 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -396,10 +385,6 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="10">
     <cellStyle name="Hiperlink" xfId="3" builtinId="8" hidden="1"/>
@@ -5271,6 +5256,296 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>513221</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>171267</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="286880" cy="530658"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Retângulo 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E29973A7-BC24-4862-AF6B-3E46B791A429}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2319161" y="5787207"/>
+          <a:ext cx="286880" cy="530658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2800" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>1</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="286880" cy="530658"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Retângulo 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9807E042-9D25-4F08-957C-3A76EEB737CD}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3992880" y="5836920"/>
+          <a:ext cx="286880" cy="530658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2800" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>3</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>220980</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="286880" cy="530658"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Retângulo 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{53BC5CC7-EB23-4FE4-8452-A2692AC2D604}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5722620" y="5836920"/>
+          <a:ext cx="286880" cy="530658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2800" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>2</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>769620</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="286880" cy="530658"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Retângulo 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{450EAF43-90B2-4578-8D6B-C134C7B34477}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5730240" y="7574280"/>
+          <a:ext cx="286880" cy="530658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2800" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>4</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>594360</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="286880" cy="530658"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Retângulo 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F552D98A-FB29-4C3A-89E7-8B78556DBD1D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3977640" y="7574280"/>
+          <a:ext cx="286880" cy="530658"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="pt-BR" sz="2800" b="0" cap="none" spc="0">
+              <a:ln w="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="38100" dist="19050" dir="2700000" algn="tl" rotWithShape="0">
+                  <a:schemeClr val="dk1">
+                    <a:alpha val="40000"/>
+                  </a:schemeClr>
+                </a:outerShdw>
+              </a:effectLst>
+            </a:rPr>
+            <a:t>5</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
@@ -5570,11 +5845,11 @@
     <tabColor theme="3" tint="0.59999389629810485"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:L13"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A9" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C6" sqref="C6:D6"/>
+      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.8984375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5591,26 +5866,26 @@
   <sheetData>
     <row r="1" spans="1:12" s="5" customFormat="1" ht="45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="6"/>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="19" t="s">
         <v>18</v>
       </c>
-      <c r="C1" s="17"/>
-      <c r="D1" s="17"/>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
     </row>
     <row r="2" spans="1:12" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="18"/>
-      <c r="C2" s="18"/>
-      <c r="D2" s="18"/>
+      <c r="B2" s="20"/>
+      <c r="C2" s="20"/>
+      <c r="D2" s="20"/>
     </row>
     <row r="3" spans="1:12" s="4" customFormat="1" ht="49.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="3"/>
       <c r="B3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="19" t="s">
+      <c r="C3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="19"/>
+      <c r="D3" s="21"/>
       <c r="E3" s="9" t="s">
         <v>2</v>
       </c>
@@ -5631,10 +5906,10 @@
       <c r="B4" s="10">
         <v>1</v>
       </c>
-      <c r="C4" s="20" t="s">
+      <c r="C4" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="21"/>
+      <c r="D4" s="23"/>
       <c r="E4" s="7">
         <v>1</v>
       </c>
@@ -5650,16 +5925,16 @@
       <c r="I4" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="23"/>
+      <c r="L4" s="17"/>
     </row>
     <row r="5" spans="1:12" ht="49.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="10">
         <v>2</v>
       </c>
-      <c r="C5" s="22" t="s">
+      <c r="C5" s="18" t="s">
         <v>10</v>
       </c>
-      <c r="D5" s="22"/>
+      <c r="D5" s="18"/>
       <c r="E5" s="7">
         <v>3</v>
       </c>
@@ -5680,10 +5955,10 @@
       <c r="B6" s="10">
         <v>3</v>
       </c>
-      <c r="C6" s="22" t="s">
+      <c r="C6" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="22"/>
+      <c r="D6" s="18"/>
       <c r="E6" s="7">
         <v>2</v>
       </c>
@@ -5704,10 +5979,10 @@
       <c r="B7" s="10">
         <v>4</v>
       </c>
-      <c r="C7" s="22" t="s">
+      <c r="C7" s="18" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="22"/>
+      <c r="D7" s="18"/>
       <c r="E7" s="7">
         <v>3</v>
       </c>
@@ -5728,10 +6003,10 @@
       <c r="B8" s="10">
         <v>5</v>
       </c>
-      <c r="C8" s="22" t="s">
+      <c r="C8" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="22"/>
+      <c r="D8" s="18"/>
       <c r="E8" s="7">
         <v>1</v>
       </c>
@@ -5762,14 +6037,14 @@
       <c r="B10" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="15" t="s">
-        <v>28</v>
+      <c r="C10" s="15">
+        <v>3</v>
       </c>
-      <c r="D10" s="16" t="s">
-        <v>30</v>
+      <c r="D10" s="16">
+        <v>6</v>
       </c>
-      <c r="E10" s="16" t="s">
-        <v>29</v>
+      <c r="E10" s="16">
+        <v>9</v>
       </c>
       <c r="F10" s="9"/>
     </row>
@@ -5787,6 +6062,7 @@
         <v>6</v>
       </c>
       <c r="F11" s="9"/>
+      <c r="I11" s="17"/>
     </row>
     <row r="12" spans="1:12" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10" t="s">
@@ -5795,19 +6071,16 @@
       <c r="C12" s="14">
         <v>1</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>32</v>
+      <c r="D12" s="14">
+        <v>2</v>
       </c>
-      <c r="E12" s="15" t="s">
-        <v>31</v>
+      <c r="E12" s="15">
+        <v>3</v>
       </c>
       <c r="F12" s="9"/>
     </row>
     <row r="13" spans="1:12" ht="70.05" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3"/>
-      <c r="B13" s="8" t="s">
-        <v>27</v>
-      </c>
       <c r="C13" s="9" t="s">
         <v>24</v>
       </c>
@@ -5818,6 +6091,17 @@
         <v>26</v>
       </c>
       <c r="F13" s="9"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="C14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="8" t="s">
+        <v>27</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -5832,6 +6116,7 @@
   </mergeCells>
   <pageMargins left="0.3" right="0.3" top="0.3" bottom="0.3" header="0" footer="0"/>
   <pageSetup scale="55" fitToHeight="0" orientation="landscape" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -5845,14 +6130,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100678EE90E01C1554D81095FA0DFA567B7" ma:contentTypeVersion="5" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="012a7ac64c29fded4fe9435d797e27e7">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="3e7a52f9-5c66-44a9-86f3-38766607b952" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="05da1342c08114b6330d010208ca11d1" ns3:_="">
     <xsd:import namespace="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
@@ -6002,6 +6279,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="3e7a52f9-5c66-44a9-86f3-38766607b952" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AD8DBBE0-27BD-4D68-870A-6C9CFB0BB6CC}">
   <ds:schemaRefs>
@@ -6011,16 +6296,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3B143F-61D5-4FE7-AF30-9937B84882D4}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2E784C7A-215E-4BC6-9503-8564823AE577}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6036,4 +6311,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BD3B143F-61D5-4FE7-AF30-9937B84882D4}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="3e7a52f9-5c66-44a9-86f3-38766607b952"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>